<commit_message>
modified to plot torques and forces as well.
</commit_message>
<xml_diff>
--- a/results_w_Activation.xlsx
+++ b/results_w_Activation.xlsx
@@ -13,7 +13,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="660">
+  <si>
+    <t>theta_h</t>
+  </si>
+  <si>
+    <t>theta_k</t>
+  </si>
+  <si>
+    <t>theta_a</t>
+  </si>
+  <si>
+    <t>f_x</t>
+  </si>
+  <si>
+    <t>f_y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>f_x_negated</t>
+  </si>
+  <si>
+    <t>f_y_negated</t>
+  </si>
+  <si>
+    <t>F_a1</t>
+  </si>
+  <si>
+    <t>F_a2</t>
+  </si>
+  <si>
+    <t>F_c1</t>
+  </si>
+  <si>
+    <t>F_c2</t>
+  </si>
+  <si>
+    <t>F_h1</t>
+  </si>
+  <si>
+    <t>F_h2</t>
+  </si>
+  <si>
+    <t>F_k1</t>
+  </si>
+  <si>
+    <t>F_k2</t>
+  </si>
+  <si>
+    <t>F_p1</t>
+  </si>
+  <si>
+    <t>F_p2</t>
+  </si>
+  <si>
+    <t>M_a3</t>
+  </si>
+  <si>
+    <t>M_h3</t>
+  </si>
+  <si>
+    <t>M_k3</t>
+  </si>
+  <si>
+    <t>M_p3</t>
+  </si>
+  <si>
+    <t>M_t3</t>
+  </si>
+  <si>
+    <t>Activation_RF</t>
+  </si>
+  <si>
+    <t>Activation_IP</t>
+  </si>
+  <si>
+    <t>Activation_G</t>
+  </si>
+  <si>
+    <t>Activation_H</t>
+  </si>
+  <si>
+    <t>Activation_TA</t>
+  </si>
+  <si>
+    <t>Activation_GA</t>
+  </si>
   <si>
     <t>theta_h</t>
   </si>
@@ -1923,7 +2013,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1938,11 +2028,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1951,6 +2042,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1963,128 +2055,128 @@
   <dimension ref="A1:AD362"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="true"/>
-    <col min="2" max="2" width="13.42578125" customWidth="true"/>
-    <col min="3" max="3" width="11.7109375" customWidth="true"/>
-    <col min="4" max="4" width="13.42578125" customWidth="true"/>
-    <col min="5" max="5" width="14.42578125" customWidth="true"/>
-    <col min="6" max="6" width="16.28515625" customWidth="true"/>
-    <col min="7" max="7" width="13.42578125" customWidth="true"/>
-    <col min="8" max="8" width="13.42578125" customWidth="true"/>
-    <col min="9" max="9" width="14.42578125" customWidth="true"/>
-    <col min="10" max="10" width="13.42578125" customWidth="true"/>
-    <col min="11" max="11" width="11.7109375" customWidth="true"/>
-    <col min="12" max="12" width="13.42578125" customWidth="true"/>
-    <col min="13" max="13" width="14.42578125" customWidth="true"/>
-    <col min="14" max="14" width="13.42578125" customWidth="true"/>
-    <col min="15" max="15" width="11.7109375" customWidth="true"/>
-    <col min="16" max="16" width="13.42578125" customWidth="true"/>
-    <col min="17" max="17" width="11.7109375" customWidth="true"/>
-    <col min="18" max="18" width="13.42578125" customWidth="true"/>
-    <col min="19" max="19" width="14.42578125" customWidth="true"/>
-    <col min="20" max="20" width="14.7109375" customWidth="true"/>
-    <col min="21" max="21" width="14.42578125" customWidth="true"/>
-    <col min="22" max="22" width="12.42578125" customWidth="true"/>
-    <col min="23" max="23" width="6" customWidth="true"/>
-    <col min="24" max="24" width="5.5703125" customWidth="true"/>
-    <col min="25" max="25" width="16.28515625" customWidth="true"/>
-    <col min="26" max="26" width="13.7109375" customWidth="true"/>
-    <col min="27" max="27" width="13.7109375" customWidth="true"/>
-    <col min="28" max="28" width="16.28515625" customWidth="true"/>
-    <col min="29" max="29" width="15.7109375" customWidth="true"/>
-    <col min="30" max="30" width="16.28515625" customWidth="true"/>
+    <col min="1" max="1" width="13.18359375" customWidth="true"/>
+    <col min="2" max="2" width="13.18359375" customWidth="true"/>
+    <col min="3" max="3" width="11.59375" customWidth="true"/>
+    <col min="4" max="4" width="13.18359375" customWidth="true"/>
+    <col min="5" max="5" width="14.18359375" customWidth="true"/>
+    <col min="6" max="6" width="15.7109375" customWidth="true"/>
+    <col min="7" max="7" width="13.18359375" customWidth="true"/>
+    <col min="8" max="8" width="13.18359375" customWidth="true"/>
+    <col min="9" max="9" width="14.18359375" customWidth="true"/>
+    <col min="10" max="10" width="13.18359375" customWidth="true"/>
+    <col min="11" max="11" width="11.59375" customWidth="true"/>
+    <col min="12" max="12" width="13.18359375" customWidth="true"/>
+    <col min="13" max="13" width="14.18359375" customWidth="true"/>
+    <col min="14" max="14" width="13.18359375" customWidth="true"/>
+    <col min="15" max="15" width="11.59375" customWidth="true"/>
+    <col min="16" max="16" width="13.18359375" customWidth="true"/>
+    <col min="17" max="17" width="11.59375" customWidth="true"/>
+    <col min="18" max="18" width="13.18359375" customWidth="true"/>
+    <col min="19" max="19" width="14.18359375" customWidth="true"/>
+    <col min="20" max="20" width="14.59375" customWidth="true"/>
+    <col min="21" max="21" width="14.18359375" customWidth="true"/>
+    <col min="22" max="22" width="12.18359375" customWidth="true"/>
+    <col min="23" max="23" width="5.7109375" customWidth="true"/>
+    <col min="24" max="24" width="5.359375" customWidth="true"/>
+    <col min="25" max="25" width="15.7109375" customWidth="true"/>
+    <col min="26" max="26" width="13.59375" customWidth="true"/>
+    <col min="27" max="27" width="13.59375" customWidth="true"/>
+    <col min="28" max="28" width="15.7109375" customWidth="true"/>
+    <col min="29" max="29" width="15.59375" customWidth="true"/>
+    <col min="30" max="30" width="15.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>601</v>
+        <v>631</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>602</v>
+        <v>632</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>603</v>
+        <v>633</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>604</v>
+        <v>634</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>605</v>
+        <v>635</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>606</v>
+        <v>636</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>607</v>
+        <v>637</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>608</v>
+        <v>638</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>609</v>
+        <v>639</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>610</v>
+        <v>640</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>611</v>
+        <v>641</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>612</v>
+        <v>642</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>613</v>
+        <v>643</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>614</v>
+        <v>644</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>615</v>
+        <v>645</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>616</v>
+        <v>646</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>617</v>
+        <v>647</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>618</v>
+        <v>648</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>619</v>
+        <v>649</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>620</v>
+        <v>650</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>621</v>
+        <v>651</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>622</v>
+        <v>652</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>623</v>
+        <v>653</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>624</v>
+        <v>654</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>625</v>
+        <v>655</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>626</v>
+        <v>656</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>627</v>
+        <v>657</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>628</v>
+        <v>658</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>629</v>
+        <v>659</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
modified bug in SymbolicEquationsOfMotion.m that had the glutes and hamstring mixed up for the torque on the knee.
</commit_message>
<xml_diff>
--- a/results_w_Activation.xlsx
+++ b/results_w_Activation.xlsx
@@ -13,7 +13,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="720">
+  <si>
+    <t>theta_h</t>
+  </si>
+  <si>
+    <t>theta_k</t>
+  </si>
+  <si>
+    <t>theta_a</t>
+  </si>
+  <si>
+    <t>f_x</t>
+  </si>
+  <si>
+    <t>f_y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>f_x_negated</t>
+  </si>
+  <si>
+    <t>f_y_negated</t>
+  </si>
+  <si>
+    <t>F_a1</t>
+  </si>
+  <si>
+    <t>F_a2</t>
+  </si>
+  <si>
+    <t>F_c1</t>
+  </si>
+  <si>
+    <t>F_c2</t>
+  </si>
+  <si>
+    <t>F_h1</t>
+  </si>
+  <si>
+    <t>F_h2</t>
+  </si>
+  <si>
+    <t>F_k1</t>
+  </si>
+  <si>
+    <t>F_k2</t>
+  </si>
+  <si>
+    <t>F_p1</t>
+  </si>
+  <si>
+    <t>F_p2</t>
+  </si>
+  <si>
+    <t>M_a3</t>
+  </si>
+  <si>
+    <t>M_h3</t>
+  </si>
+  <si>
+    <t>M_k3</t>
+  </si>
+  <si>
+    <t>M_p3</t>
+  </si>
+  <si>
+    <t>M_t3</t>
+  </si>
+  <si>
+    <t>Activation_RF</t>
+  </si>
+  <si>
+    <t>Activation_IP</t>
+  </si>
+  <si>
+    <t>Activation_G</t>
+  </si>
+  <si>
+    <t>Activation_H</t>
+  </si>
+  <si>
+    <t>Activation_TA</t>
+  </si>
+  <si>
+    <t>Activation_GA</t>
+  </si>
   <si>
     <t>theta_h</t>
   </si>
@@ -2103,7 +2193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2120,11 +2210,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -2135,6 +2226,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2173,102 +2265,102 @@
     <col min="24" max="24" width="5.359375" customWidth="true"/>
     <col min="25" max="25" width="12.59375" customWidth="true"/>
     <col min="26" max="26" width="12.59375" customWidth="true"/>
-    <col min="27" max="27" width="12.59375" customWidth="true"/>
-    <col min="28" max="28" width="11.30078125" customWidth="true"/>
+    <col min="27" max="27" width="11.30078125" customWidth="true"/>
+    <col min="28" max="28" width="12.59375" customWidth="true"/>
     <col min="29" max="29" width="12.59375" customWidth="true"/>
     <col min="30" max="30" width="12.41796875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>660</v>
+        <v>690</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>661</v>
+        <v>691</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>662</v>
+        <v>692</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>663</v>
+        <v>693</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>664</v>
+        <v>694</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>665</v>
+        <v>695</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>666</v>
+        <v>696</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>667</v>
+        <v>697</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>668</v>
+        <v>698</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>669</v>
+        <v>699</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>670</v>
+        <v>700</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>671</v>
+        <v>701</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>672</v>
+        <v>702</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>673</v>
+        <v>703</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>674</v>
+        <v>704</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>675</v>
+        <v>705</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>676</v>
+        <v>706</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>677</v>
+        <v>707</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>678</v>
+        <v>708</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>679</v>
+        <v>709</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>680</v>
+        <v>710</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>681</v>
+        <v>711</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>682</v>
+        <v>712</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>683</v>
+        <v>713</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>684</v>
+        <v>714</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>685</v>
+        <v>715</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>686</v>
+        <v>716</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>687</v>
+        <v>717</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>688</v>
+        <v>718</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>689</v>
+        <v>719</v>
       </c>
     </row>
     <row r="2">
@@ -2345,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="Y2" s="0">
-        <v>0.17698841486691094</v>
+        <v>0.17698841486691091</v>
       </c>
       <c r="Z2" s="0">
         <v>0.32339390803646673</v>
@@ -2529,10 +2621,10 @@
         <v>0</v>
       </c>
       <c r="Y4" s="0">
-        <v>0.16842111844880656</v>
+        <v>0.16842111844880653</v>
       </c>
       <c r="Z4" s="0">
-        <v>0.33614648194357472</v>
+        <v>0.33614648194357477</v>
       </c>
       <c r="AA4" s="0">
         <v>0.10000000000000001</v>
@@ -2713,10 +2805,10 @@
         <v>0</v>
       </c>
       <c r="Y6" s="0">
-        <v>0.16166329703222757</v>
+        <v>0.16166329703222754</v>
       </c>
       <c r="Z6" s="0">
-        <v>0.34576663329448609</v>
+        <v>0.34576663329448615</v>
       </c>
       <c r="AA6" s="0">
         <v>0.10000000000000001</v>
@@ -2725,7 +2817,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC6" s="0">
-        <v>0.1638561189135764</v>
+        <v>0.16385611891357643</v>
       </c>
       <c r="AD6" s="0">
         <v>0.10000000000000001</v>
@@ -2808,7 +2900,7 @@
         <v>0.15831495216660524</v>
       </c>
       <c r="Z7" s="0">
-        <v>0.35028193351099784</v>
+        <v>0.35028193351099779</v>
       </c>
       <c r="AA7" s="0">
         <v>0.10000000000000001</v>
@@ -3084,7 +3176,7 @@
         <v>0.14688096327487093</v>
       </c>
       <c r="Z10" s="0">
-        <v>0.36565062574790486</v>
+        <v>0.3656506257479048</v>
       </c>
       <c r="AA10" s="0">
         <v>0.10000000000000001</v>
@@ -3268,7 +3360,7 @@
         <v>0.13709603861550856</v>
       </c>
       <c r="Z12" s="0">
-        <v>0.37807181948837298</v>
+        <v>0.37807181948837293</v>
       </c>
       <c r="AA12" s="0">
         <v>0.10000000000000001</v>
@@ -4007,10 +4099,10 @@
         <v>0.42627142517971583</v>
       </c>
       <c r="AA20" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB20" s="0">
         <v>0.10135096070710282</v>
-      </c>
-      <c r="AB20" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC20" s="0">
         <v>0.19943476547219852</v>
@@ -4096,13 +4188,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z21" s="0">
-        <v>0.43311474350976564</v>
+        <v>0.43311474350976559</v>
       </c>
       <c r="AA21" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB21" s="0">
         <v>0.10374542631422169</v>
-      </c>
-      <c r="AB21" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC21" s="0">
         <v>0.2025030732397286</v>
@@ -4191,10 +4283,10 @@
         <v>0.4391299858474908</v>
       </c>
       <c r="AA22" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB22" s="0">
         <v>0.10590115703973922</v>
-      </c>
-      <c r="AB22" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC22" s="0">
         <v>0.20518359749037382</v>
@@ -4283,13 +4375,13 @@
         <v>0.4460027405376441</v>
       </c>
       <c r="AA23" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB23" s="0">
         <v>0.10827837237849869</v>
       </c>
-      <c r="AB23" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC23" s="0">
-        <v>0.20832639769669967</v>
+        <v>0.20832639769669964</v>
       </c>
       <c r="AD23" s="0">
         <v>0.10000000000000001</v>
@@ -4372,13 +4464,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z24" s="0">
-        <v>0.4530938735255402</v>
+        <v>0.45309387352554015</v>
       </c>
       <c r="AA24" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB24" s="0">
         <v>0.11085997711898256</v>
-      </c>
-      <c r="AB24" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC24" s="0">
         <v>0.21152340865300717</v>
@@ -4467,10 +4559,10 @@
         <v>0.46013119378525869</v>
       </c>
       <c r="AA25" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB25" s="0">
         <v>0.11344680214054056</v>
-      </c>
-      <c r="AB25" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC25" s="0">
         <v>0.21470408278391537</v>
@@ -4559,10 +4651,10 @@
         <v>0.4671528133670258</v>
       </c>
       <c r="AA26" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB26" s="0">
         <v>0.11615897951380606</v>
-      </c>
-      <c r="AB26" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC26" s="0">
         <v>0.21783117938950491</v>
@@ -4648,13 +4740,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z27" s="0">
-        <v>0.47354303047981555</v>
+        <v>0.47354303047981561</v>
       </c>
       <c r="AA27" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB27" s="0">
         <v>0.11857100067454367</v>
-      </c>
-      <c r="AB27" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC27" s="0">
         <v>0.22073677641859885</v>
@@ -4740,13 +4832,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z28" s="0">
-        <v>0.48061982998688518</v>
+        <v>0.48061982998688524</v>
       </c>
       <c r="AA28" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB28" s="0">
         <v>0.1213020374601691</v>
-      </c>
-      <c r="AB28" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC28" s="0">
         <v>0.22394925502879107</v>
@@ -4835,10 +4927,10 @@
         <v>0.48728979611356377</v>
       </c>
       <c r="AA29" s="0">
-        <v>0.12379988287949813</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB29" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.12379988287949811</v>
       </c>
       <c r="AC29" s="0">
         <v>0.22704270070425889</v>
@@ -4924,13 +5016,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z30" s="0">
-        <v>0.49508880684164108</v>
+        <v>0.49508880684164119</v>
       </c>
       <c r="AA30" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB30" s="0">
         <v>0.12681628875850165</v>
-      </c>
-      <c r="AB30" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC30" s="0">
         <v>0.23063694877007709</v>
@@ -5019,10 +5111,10 @@
         <v>0.50187039981815518</v>
       </c>
       <c r="AA31" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB31" s="0">
         <v>0.1295008952298681</v>
-      </c>
-      <c r="AB31" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC31" s="0">
         <v>0.23377333595279845</v>
@@ -5108,13 +5200,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z32" s="0">
-        <v>0.50794810606773577</v>
+        <v>0.50794810606773588</v>
       </c>
       <c r="AA32" s="0">
-        <v>0.13193312930203832</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB32" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.13193312930203835</v>
       </c>
       <c r="AC32" s="0">
         <v>0.23660263133333856</v>
@@ -5203,10 +5295,10 @@
         <v>0.51460232997794431</v>
       </c>
       <c r="AA33" s="0">
-        <v>0.13469075262532854</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB33" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.13469075262532856</v>
       </c>
       <c r="AC33" s="0">
         <v>0.23967959423825533</v>
@@ -5295,10 +5387,10 @@
         <v>0.52279693637835145</v>
       </c>
       <c r="AA34" s="0">
-        <v>0.13794807130463263</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB34" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.13794807130463266</v>
       </c>
       <c r="AC34" s="0">
         <v>0.24355293425454791</v>
@@ -5387,10 +5479,10 @@
         <v>0.53017047986960941</v>
       </c>
       <c r="AA35" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB35" s="0">
         <v>0.14097449022800973</v>
-      </c>
-      <c r="AB35" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC35" s="0">
         <v>0.24703857195930115</v>
@@ -5476,13 +5568,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z36" s="0">
-        <v>0.53655521712135812</v>
+        <v>0.53655521712135823</v>
       </c>
       <c r="AA36" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB36" s="0">
         <v>0.14372177918181872</v>
-      </c>
-      <c r="AB36" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC36" s="0">
         <v>0.25005570499636165</v>
@@ -5571,10 +5663,10 @@
         <v>0.54327949988683166</v>
       </c>
       <c r="AA37" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB37" s="0">
         <v>0.14647123447814331</v>
-      </c>
-      <c r="AB37" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC37" s="0">
         <v>0.25332547145672757</v>
@@ -5660,13 +5752,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z38" s="0">
-        <v>0.5508525840203814</v>
+        <v>0.55085258402038129</v>
       </c>
       <c r="AA38" s="0">
-        <v>0.14968730134901778</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB38" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.14968730134901781</v>
       </c>
       <c r="AC38" s="0">
         <v>0.25697213205028868</v>
@@ -5755,10 +5847,10 @@
         <v>0.55665788254280479</v>
       </c>
       <c r="AA39" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB39" s="0">
         <v>0.15221090816341271</v>
-      </c>
-      <c r="AB39" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC39" s="0">
         <v>0.25982711412366477</v>
@@ -5844,16 +5936,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z40" s="0">
-        <v>0.562924570795301</v>
+        <v>0.56292457079530112</v>
       </c>
       <c r="AA40" s="0">
+        <v>0.10000000000000002</v>
+      </c>
+      <c r="AB40" s="0">
         <v>0.15494036197321698</v>
       </c>
-      <c r="AB40" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC40" s="0">
-        <v>0.26292424058824365</v>
+        <v>0.26292424058824371</v>
       </c>
       <c r="AD40" s="0">
         <v>0.10000000000000001</v>
@@ -5936,13 +6028,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z41" s="0">
-        <v>0.57015694280416196</v>
+        <v>0.57015694280416185</v>
       </c>
       <c r="AA41" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB41" s="0">
         <v>0.15821782491917463</v>
-      </c>
-      <c r="AB41" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC41" s="0">
         <v>0.26644669698195844</v>
@@ -6028,13 +6120,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z42" s="0">
-        <v>0.5764906190704896</v>
+        <v>0.57649061907048949</v>
       </c>
       <c r="AA42" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB42" s="0">
         <v>0.16094934454678636</v>
-      </c>
-      <c r="AB42" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC42" s="0">
         <v>0.26966730808494871</v>
@@ -6120,13 +6212,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z43" s="0">
-        <v>0.58249537286056274</v>
+        <v>0.58249537286056285</v>
       </c>
       <c r="AA43" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB43" s="0">
         <v>0.16355305800471664</v>
-      </c>
-      <c r="AB43" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC43" s="0">
         <v>0.27276934278166015</v>
@@ -6215,10 +6307,10 @@
         <v>0.58843408290648724</v>
       </c>
       <c r="AA44" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB44" s="0">
         <v>0.16632908418564504</v>
-      </c>
-      <c r="AB44" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC44" s="0">
         <v>0.2757959701361461</v>
@@ -6307,10 +6399,10 @@
         <v>0.59440561114324608</v>
       </c>
       <c r="AA45" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB45" s="0">
         <v>0.16905619519014939</v>
-      </c>
-      <c r="AB45" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC45" s="0">
         <v>0.27890319942894787</v>
@@ -6396,13 +6488,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z46" s="0">
-        <v>0.60031694613737863</v>
+        <v>0.60031694613737874</v>
       </c>
       <c r="AA46" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB46" s="0">
         <v>0.17179031020753635</v>
-      </c>
-      <c r="AB46" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC46" s="0">
         <v>0.28201569588086844</v>
@@ -6491,10 +6583,10 @@
         <v>0.60705536804195648</v>
       </c>
       <c r="AA47" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB47" s="0">
         <v>0.17500804969974398</v>
-      </c>
-      <c r="AB47" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC47" s="0">
         <v>0.28551039457533595</v>
@@ -6583,10 +6675,10 @@
         <v>0.61209308796034534</v>
       </c>
       <c r="AA48" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB48" s="0">
         <v>0.17730085738263207</v>
-      </c>
-      <c r="AB48" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC48" s="0">
         <v>0.28832114012848653</v>
@@ -6672,16 +6764,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z49" s="0">
-        <v>0.61703171750468211</v>
+        <v>0.61703171750468233</v>
       </c>
       <c r="AA49" s="0">
-        <v>0.17965899096895302</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB49" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.17965899096895305</v>
       </c>
       <c r="AC49" s="0">
-        <v>0.29108333061753766</v>
+        <v>0.29108333061753772</v>
       </c>
       <c r="AD49" s="0">
         <v>0.10000000000000001</v>
@@ -6767,10 +6859,10 @@
         <v>0.62300055380400365</v>
       </c>
       <c r="AA50" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB50" s="0">
         <v>0.18238286194073744</v>
-      </c>
-      <c r="AB50" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC50" s="0">
         <v>0.29440546397678047</v>
@@ -6859,10 +6951,10 @@
         <v>0.63033790854685601</v>
       </c>
       <c r="AA51" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB51" s="0">
         <v>0.18607889685985207</v>
-      </c>
-      <c r="AB51" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC51" s="0">
         <v>0.29829279890392235</v>
@@ -6951,10 +7043,10 @@
         <v>0.63528748383561096</v>
       </c>
       <c r="AA52" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB52" s="0">
         <v>0.1882838662157936</v>
-      </c>
-      <c r="AB52" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC52" s="0">
         <v>0.30124867947420403</v>
@@ -7040,13 +7132,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z53" s="0">
-        <v>0.63918464965358879</v>
+        <v>0.63918464965358868</v>
       </c>
       <c r="AA53" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB53" s="0">
         <v>0.19032927829018043</v>
-      </c>
-      <c r="AB53" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC53" s="0">
         <v>0.30363897561135927</v>
@@ -7135,10 +7227,10 @@
         <v>0.64296308589324369</v>
       </c>
       <c r="AA54" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB54" s="0">
         <v>0.19213513195866633</v>
-      </c>
-      <c r="AB54" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC54" s="0">
         <v>0.30607238179518609</v>
@@ -7227,10 +7319,10 @@
         <v>0.64731395740826636</v>
       </c>
       <c r="AA55" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB55" s="0">
         <v>0.19442165141254394</v>
-      </c>
-      <c r="AB55" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC55" s="0">
         <v>0.30874791281259295</v>
@@ -7316,13 +7408,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z56" s="0">
-        <v>0.65124932574807237</v>
+        <v>0.65124932574807248</v>
       </c>
       <c r="AA56" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB56" s="0">
         <v>0.19645153611510149</v>
-      </c>
-      <c r="AB56" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC56" s="0">
         <v>0.31129421731354739</v>
@@ -7411,10 +7503,10 @@
         <v>0.65531550391903182</v>
       </c>
       <c r="AA57" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB57" s="0">
         <v>0.19836153498226569</v>
-      </c>
-      <c r="AB57" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC57" s="0">
         <v>0.31399676003165572</v>
@@ -7503,10 +7595,10 @@
         <v>0.66120622259886985</v>
       </c>
       <c r="AA58" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB58" s="0">
         <v>0.20143830612768282</v>
-      </c>
-      <c r="AB58" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC58" s="0">
         <v>0.31752827094864666</v>
@@ -7595,10 +7687,10 @@
         <v>0.66476805613909651</v>
       </c>
       <c r="AA59" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB59" s="0">
         <v>0.20317313439228205</v>
-      </c>
-      <c r="AB59" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC59" s="0">
         <v>0.32005840579200168</v>
@@ -7687,10 +7779,10 @@
         <v>0.6684695894281143</v>
       </c>
       <c r="AA60" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB60" s="0">
         <v>0.2050779077008193</v>
-      </c>
-      <c r="AB60" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC60" s="0">
         <v>0.32266920387249676</v>
@@ -7776,13 +7868,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z61" s="0">
-        <v>0.67346242088237729</v>
+        <v>0.67346242088237718</v>
       </c>
       <c r="AA61" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB61" s="0">
         <v>0.2077588278566645</v>
-      </c>
-      <c r="AB61" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC61" s="0">
         <v>0.32590443022863802</v>
@@ -7871,10 +7963,10 @@
         <v>0.67714439877836319</v>
       </c>
       <c r="AA62" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB62" s="0">
         <v>0.20985807811304236</v>
-      </c>
-      <c r="AB62" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC62" s="0">
         <v>0.32854731705576307</v>
@@ -7960,13 +8052,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z63" s="0">
-        <v>0.67978459937974745</v>
+        <v>0.67978459937974756</v>
       </c>
       <c r="AA63" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB63" s="0">
         <v>0.21114734054886491</v>
-      </c>
-      <c r="AB63" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC63" s="0">
         <v>0.33081360340053351</v>
@@ -8055,10 +8147,10 @@
         <v>0.68292184931955791</v>
       </c>
       <c r="AA64" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB64" s="0">
         <v>0.21291376670324402</v>
-      </c>
-      <c r="AB64" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC64" s="0">
         <v>0.33330039402522332</v>
@@ -8147,10 +8239,10 @@
         <v>0.68609575402700695</v>
       </c>
       <c r="AA65" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB65" s="0">
         <v>0.21460859670740737</v>
-      </c>
-      <c r="AB65" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC65" s="0">
         <v>0.33587884504718107</v>
@@ -8239,10 +8331,10 @@
         <v>0.68897698044483335</v>
       </c>
       <c r="AA66" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB66" s="0">
         <v>0.21629649023863295</v>
-      </c>
-      <c r="AB66" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC66" s="0">
         <v>0.33832794651783504</v>
@@ -8331,10 +8423,10 @@
         <v>0.69077995534432823</v>
       </c>
       <c r="AA67" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB67" s="0">
         <v>0.21765173756179176</v>
-      </c>
-      <c r="AB67" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC67" s="0">
         <v>0.34023836506914829</v>
@@ -8423,10 +8515,10 @@
         <v>0.69244801457140004</v>
       </c>
       <c r="AA68" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB68" s="0">
         <v>0.21852503743996377</v>
-      </c>
-      <c r="AB68" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC68" s="0">
         <v>0.34223006883663598</v>
@@ -8515,10 +8607,10 @@
         <v>0.6949352103290799</v>
       </c>
       <c r="AA69" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB69" s="0">
         <v>0.22032806155093157</v>
-      </c>
-      <c r="AB69" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC69" s="0">
         <v>0.34454963520397708</v>
@@ -8607,10 +8699,10 @@
         <v>0.696427969122423</v>
       </c>
       <c r="AA70" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB70" s="0">
         <v>0.22137207865435751</v>
-      </c>
-      <c r="AB70" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC70" s="0">
         <v>0.34648186302189704</v>
@@ -8696,13 +8788,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z71" s="0">
-        <v>0.69690329383412541</v>
+        <v>0.69690329383412553</v>
       </c>
       <c r="AA71" s="0">
-        <v>0.22176300329279011</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB71" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.22176300329279008</v>
       </c>
       <c r="AC71" s="0">
         <v>0.34797817154894756</v>
@@ -8791,10 +8883,10 @@
         <v>0.69777900734854781</v>
       </c>
       <c r="AA72" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB72" s="0">
         <v>0.22279166248970037</v>
-      </c>
-      <c r="AB72" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC72" s="0">
         <v>0.3496139353294872</v>
@@ -8883,10 +8975,10 @@
         <v>0.69844026112998669</v>
       </c>
       <c r="AA73" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB73" s="0">
         <v>0.22352733816913373</v>
-      </c>
-      <c r="AB73" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC73" s="0">
         <v>0.35122845031240885</v>
@@ -8975,10 +9067,10 @@
         <v>0.69843193153677297</v>
       </c>
       <c r="AA74" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB74" s="0">
         <v>0.22374028945410881</v>
-      </c>
-      <c r="AB74" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC74" s="0">
         <v>0.35258481853688861</v>
@@ -9067,10 +9159,10 @@
         <v>0.69860296550949608</v>
       </c>
       <c r="AA75" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB75" s="0">
         <v>0.22429344182350494</v>
-      </c>
-      <c r="AB75" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC75" s="0">
         <v>0.35401627761040816</v>
@@ -9159,10 +9251,10 @@
         <v>0.6984908179496655</v>
       </c>
       <c r="AA76" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB76" s="0">
         <v>0.22471277269964582</v>
-      </c>
-      <c r="AB76" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC76" s="0">
         <v>0.3553400832644692</v>
@@ -9251,10 +9343,10 @@
         <v>0.69800392633081154</v>
       </c>
       <c r="AA77" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB77" s="0">
         <v>0.2251745917043072</v>
-      </c>
-      <c r="AB77" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC77" s="0">
         <v>0.35645357242424525</v>
@@ -9343,10 +9435,10 @@
         <v>0.69738514620216807</v>
       </c>
       <c r="AA78" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB78" s="0">
         <v>0.2253453910310465</v>
-      </c>
-      <c r="AB78" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC78" s="0">
         <v>0.3575835529697769</v>
@@ -9435,10 +9527,10 @@
         <v>0.69684450946403242</v>
       </c>
       <c r="AA79" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB79" s="0">
         <v>0.22560107029641016</v>
-      </c>
-      <c r="AB79" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC79" s="0">
         <v>0.35879441259264944</v>
@@ -9527,10 +9619,10 @@
         <v>0.69626727349995909</v>
       </c>
       <c r="AA80" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB80" s="0">
         <v>0.22587979154373167</v>
-      </c>
-      <c r="AB80" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC80" s="0">
         <v>0.36001058310953854</v>
@@ -9616,13 +9708,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z81" s="0">
-        <v>0.69558652981977431</v>
+        <v>0.69558652981977442</v>
       </c>
       <c r="AA81" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB81" s="0">
         <v>0.226301199949732</v>
-      </c>
-      <c r="AB81" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC81" s="0">
         <v>0.36117815082794352</v>
@@ -9711,10 +9803,10 @@
         <v>0.69475847834165527</v>
       </c>
       <c r="AA82" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB82" s="0">
         <v>0.22669399643507024</v>
-      </c>
-      <c r="AB82" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC82" s="0">
         <v>0.36229723996167268</v>
@@ -9803,10 +9895,10 @@
         <v>0.69379785603136934</v>
       </c>
       <c r="AA83" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB83" s="0">
         <v>0.22673948490200882</v>
-      </c>
-      <c r="AB83" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC83" s="0">
         <v>0.36344376745045198</v>
@@ -9895,10 +9987,10 @@
         <v>0.69201576813808929</v>
       </c>
       <c r="AA84" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB84" s="0">
         <v>0.22642298418865583</v>
-      </c>
-      <c r="AB84" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC84" s="0">
         <v>0.36415393743131846</v>
@@ -9987,10 +10079,10 @@
         <v>0.6905603152552573</v>
       </c>
       <c r="AA85" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB85" s="0">
         <v>0.22646009371920753</v>
-      </c>
-      <c r="AB85" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC85" s="0">
         <v>0.36504704160839696</v>
@@ -10079,13 +10171,13 @@
         <v>0.68884638513232188</v>
       </c>
       <c r="AA86" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB86" s="0">
         <v>0.22653363476249214</v>
       </c>
-      <c r="AB86" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC86" s="0">
-        <v>0.36579992822281587</v>
+        <v>0.36579992822281593</v>
       </c>
       <c r="AD86" s="0">
         <v>0.10000000000000001</v>
@@ -10171,13 +10263,13 @@
         <v>0.68709470997193378</v>
       </c>
       <c r="AA87" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB87" s="0">
         <v>0.22657750456066794</v>
       </c>
-      <c r="AB87" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC87" s="0">
-        <v>0.36656902197776042</v>
+        <v>0.36656902197776031</v>
       </c>
       <c r="AD87" s="0">
         <v>0.10000000000000001</v>
@@ -10263,10 +10355,10 @@
         <v>0.68493685892479805</v>
       </c>
       <c r="AA88" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB88" s="0">
         <v>0.22612253469340868</v>
-      </c>
-      <c r="AB88" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC88" s="0">
         <v>0.36719859876104544</v>
@@ -10355,10 +10447,10 @@
         <v>0.68296917779984412</v>
       </c>
       <c r="AA89" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB89" s="0">
         <v>0.22616969752712995</v>
-      </c>
-      <c r="AB89" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC89" s="0">
         <v>0.36789767106983362</v>
@@ -10447,10 +10539,10 @@
         <v>0.68070267605699475</v>
       </c>
       <c r="AA90" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB90" s="0">
         <v>0.22572862296760909</v>
-      </c>
-      <c r="AB90" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC90" s="0">
         <v>0.36852192574424009</v>
@@ -10539,10 +10631,10 @@
         <v>0.67836065248905464</v>
       </c>
       <c r="AA91" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB91" s="0">
         <v>0.22557757109544416</v>
-      </c>
-      <c r="AB91" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC91" s="0">
         <v>0.36908119781553217</v>
@@ -10631,10 +10723,10 @@
         <v>0.67587325770761852</v>
       </c>
       <c r="AA92" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB92" s="0">
         <v>0.22540193196498645</v>
-      </c>
-      <c r="AB92" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC92" s="0">
         <v>0.36958123044172303</v>
@@ -10720,13 +10812,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z93" s="0">
-        <v>0.67299614060819313</v>
+        <v>0.67299614060819324</v>
       </c>
       <c r="AA93" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB93" s="0">
         <v>0.22485220493713803</v>
-      </c>
-      <c r="AB93" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC93" s="0">
         <v>0.36990917119603756</v>
@@ -10812,16 +10904,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z94" s="0">
-        <v>0.67019519067805744</v>
+        <v>0.67019519067805733</v>
       </c>
       <c r="AA94" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB94" s="0">
         <v>0.22453702949534199</v>
       </c>
-      <c r="AB94" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC94" s="0">
-        <v>0.37029095385489813</v>
+        <v>0.37029095385489808</v>
       </c>
       <c r="AD94" s="0">
         <v>0.10000000000000001</v>
@@ -10907,10 +10999,10 @@
         <v>0.66710458754449597</v>
       </c>
       <c r="AA95" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB95" s="0">
         <v>0.22428345870081612</v>
-      </c>
-      <c r="AB95" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC95" s="0">
         <v>0.37048927468292475</v>
@@ -10999,10 +11091,10 @@
         <v>0.66375450264804259</v>
       </c>
       <c r="AA96" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB96" s="0">
         <v>0.22347400436735818</v>
-      </c>
-      <c r="AB96" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC96" s="0">
         <v>0.37062358397995299</v>
@@ -11091,10 +11183,10 @@
         <v>0.66041227934512836</v>
       </c>
       <c r="AA97" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB97" s="0">
         <v>0.22320952958822071</v>
-      </c>
-      <c r="AB97" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC97" s="0">
         <v>0.37070881124387689</v>
@@ -11183,10 +11275,10 @@
         <v>0.6567618136047878</v>
       </c>
       <c r="AA98" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB98" s="0">
         <v>0.22245660970834463</v>
-      </c>
-      <c r="AB98" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC98" s="0">
         <v>0.37068696114894067</v>
@@ -11272,16 +11364,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z99" s="0">
-        <v>0.65314729945821703</v>
+        <v>0.65314729945821715</v>
       </c>
       <c r="AA99" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB99" s="0">
         <v>0.22227797460248214</v>
       </c>
-      <c r="AB99" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC99" s="0">
-        <v>0.37063217177906466</v>
+        <v>0.37063217177906471</v>
       </c>
       <c r="AD99" s="0">
         <v>0.10000000000000001</v>
@@ -11364,13 +11456,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z100" s="0">
-        <v>0.64913202695454686</v>
+        <v>0.64913202695454675</v>
       </c>
       <c r="AA100" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB100" s="0">
         <v>0.22170285122288461</v>
-      </c>
-      <c r="AB100" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC100" s="0">
         <v>0.37038392350279381</v>
@@ -11459,10 +11551,10 @@
         <v>0.64508024130725139</v>
       </c>
       <c r="AA101" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB101" s="0">
         <v>0.22107362872829359</v>
-      </c>
-      <c r="AB101" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC101" s="0">
         <v>0.37012474091365799</v>
@@ -11548,13 +11640,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z102" s="0">
-        <v>0.64090911420429963</v>
+        <v>0.64090911420429975</v>
       </c>
       <c r="AA102" s="0">
-        <v>0.22020817759804154</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB102" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.22020817759804157</v>
       </c>
       <c r="AC102" s="0">
         <v>0.36983356806939571</v>
@@ -11643,13 +11735,13 @@
         <v>0.63646658200800543</v>
       </c>
       <c r="AA103" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB103" s="0">
         <v>0.21938306885702388</v>
       </c>
-      <c r="AB103" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC103" s="0">
-        <v>0.36937008536908228</v>
+        <v>0.36937008536908233</v>
       </c>
       <c r="AD103" s="0">
         <v>0.10000000000000001</v>
@@ -11735,10 +11827,10 @@
         <v>0.63188926194105577</v>
       </c>
       <c r="AA104" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB104" s="0">
         <v>0.21884160859263055</v>
-      </c>
-      <c r="AB104" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC104" s="0">
         <v>0.3687821796005713</v>
@@ -11824,13 +11916,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z105" s="0">
-        <v>0.62731708488625026</v>
+        <v>0.62731708488625015</v>
       </c>
       <c r="AA105" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB105" s="0">
         <v>0.21797543912546841</v>
-      </c>
-      <c r="AB105" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC105" s="0">
         <v>0.36824852368771305</v>
@@ -11919,10 +12011,10 @@
         <v>0.62256927059314926</v>
       </c>
       <c r="AA106" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB106" s="0">
         <v>0.21674329448185653</v>
-      </c>
-      <c r="AB106" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC106" s="0">
         <v>0.36765083138002075</v>
@@ -12011,10 +12103,10 @@
         <v>0.61732135713932945</v>
       </c>
       <c r="AA107" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB107" s="0">
         <v>0.21594962713121338</v>
-      </c>
-      <c r="AB107" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC107" s="0">
         <v>0.36665401064192249</v>
@@ -12100,13 +12192,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z108" s="0">
-        <v>0.61197452714395728</v>
+        <v>0.61197452714395717</v>
       </c>
       <c r="AA108" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB108" s="0">
         <v>0.21514207046013681</v>
-      </c>
-      <c r="AB108" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC108" s="0">
         <v>0.36558709992748117</v>
@@ -12195,10 +12287,10 @@
         <v>0.60639369430750023</v>
       </c>
       <c r="AA109" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB109" s="0">
         <v>0.21410168508943836</v>
-      </c>
-      <c r="AB109" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC109" s="0">
         <v>0.36438052257320036</v>
@@ -12287,10 +12379,10 @@
         <v>0.60121501510689335</v>
       </c>
       <c r="AA110" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB110" s="0">
         <v>0.21311305368032527</v>
-      </c>
-      <c r="AB110" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC110" s="0">
         <v>0.36344838757014847</v>
@@ -12379,10 +12471,10 @@
         <v>0.59577832138826514</v>
       </c>
       <c r="AA111" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB111" s="0">
         <v>0.21189052507507086</v>
-      </c>
-      <c r="AB111" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC111" s="0">
         <v>0.36235505369014037</v>
@@ -12471,10 +12563,10 @@
         <v>0.59037954083228117</v>
       </c>
       <c r="AA112" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB112" s="0">
         <v>0.21081430544080845</v>
-      </c>
-      <c r="AB112" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC112" s="0">
         <v>0.36126684513565321</v>
@@ -12563,10 +12655,10 @@
         <v>0.58478907060292196</v>
       </c>
       <c r="AA113" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB113" s="0">
         <v>0.20981893392579368</v>
-      </c>
-      <c r="AB113" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC113" s="0">
         <v>0.36002230581490419</v>
@@ -12652,13 +12744,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z114" s="0">
-        <v>0.57923575588144727</v>
+        <v>0.57923575588144716</v>
       </c>
       <c r="AA114" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB114" s="0">
         <v>0.20900139838462237</v>
-      </c>
-      <c r="AB114" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC114" s="0">
         <v>0.35877740954664727</v>
@@ -12747,10 +12839,10 @@
         <v>0.57354130947044668</v>
       </c>
       <c r="AA115" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB115" s="0">
         <v>0.20769513263469086</v>
-      </c>
-      <c r="AB115" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC115" s="0">
         <v>0.35746868353678174</v>
@@ -12836,13 +12928,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z116" s="0">
-        <v>0.56753517185853952</v>
+        <v>0.56753517185853941</v>
       </c>
       <c r="AA116" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB116" s="0">
         <v>0.20629805296933323</v>
-      </c>
-      <c r="AB116" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC116" s="0">
         <v>0.35591773756008527</v>
@@ -12931,10 +13023,10 @@
         <v>0.56136243292239674</v>
       </c>
       <c r="AA117" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB117" s="0">
         <v>0.20519408319675791</v>
-      </c>
-      <c r="AB117" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC117" s="0">
         <v>0.35418847639216289</v>
@@ -13020,13 +13112,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z118" s="0">
-        <v>0.55547673717456425</v>
+        <v>0.55547673717456414</v>
       </c>
       <c r="AA118" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB118" s="0">
         <v>0.20383162236950186</v>
-      </c>
-      <c r="AB118" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC118" s="0">
         <v>0.3526859006031875</v>
@@ -13115,10 +13207,10 @@
         <v>0.54920545304829826</v>
       </c>
       <c r="AA119" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB119" s="0">
         <v>0.20269024443364464</v>
-      </c>
-      <c r="AB119" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC119" s="0">
         <v>0.35083816857674849</v>
@@ -13204,13 +13296,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z120" s="0">
-        <v>0.54327611986505375</v>
+        <v>0.54327611986505386</v>
       </c>
       <c r="AA120" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB120" s="0">
         <v>0.20108819267432593</v>
-      </c>
-      <c r="AB120" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC120" s="0">
         <v>0.34927672034359858</v>
@@ -13299,10 +13391,10 @@
         <v>0.53720746496837068</v>
       </c>
       <c r="AA121" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB121" s="0">
         <v>0.19970227913801869</v>
-      </c>
-      <c r="AB121" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC121" s="0">
         <v>0.34755866660475454</v>
@@ -13391,10 +13483,10 @@
         <v>0.53125873568586246</v>
       </c>
       <c r="AA122" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB122" s="0">
         <v>0.19843566614640115</v>
-      </c>
-      <c r="AB122" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC122" s="0">
         <v>0.34589966033182545</v>
@@ -13483,13 +13575,13 @@
         <v>0.52529165301429037</v>
       </c>
       <c r="AA123" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB123" s="0">
         <v>0.1968372588284043</v>
       </c>
-      <c r="AB123" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC123" s="0">
-        <v>0.34422504494721012</v>
+        <v>0.34422504494721018</v>
       </c>
       <c r="AD123" s="0">
         <v>0.10000000000000001</v>
@@ -13575,10 +13667,10 @@
         <v>0.51931098368475215</v>
       </c>
       <c r="AA124" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB124" s="0">
         <v>0.19558635721549864</v>
-      </c>
-      <c r="AB124" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC124" s="0">
         <v>0.342479790115024</v>
@@ -13667,10 +13759,10 @@
         <v>0.51307801043258328</v>
       </c>
       <c r="AA125" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB125" s="0">
         <v>0.19423418779903889</v>
-      </c>
-      <c r="AB125" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC125" s="0">
         <v>0.34049760798095074</v>
@@ -13759,13 +13851,13 @@
         <v>0.5069245522151149</v>
       </c>
       <c r="AA126" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB126" s="0">
         <v>0.19239488090154613</v>
       </c>
-      <c r="AB126" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC126" s="0">
-        <v>0.33858105323419141</v>
+        <v>0.33858105323419146</v>
       </c>
       <c r="AD126" s="0">
         <v>0.10000000000000001</v>
@@ -13851,10 +13943,10 @@
         <v>0.50108690441795034</v>
       </c>
       <c r="AA127" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB127" s="0">
         <v>0.19127321191024627</v>
-      </c>
-      <c r="AB127" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC127" s="0">
         <v>0.3368408990534828</v>
@@ -13940,13 +14032,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z128" s="0">
-        <v>0.49548586696688607</v>
+        <v>0.49548586696688612</v>
       </c>
       <c r="AA128" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB128" s="0">
         <v>0.18982523754452219</v>
-      </c>
-      <c r="AB128" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC128" s="0">
         <v>0.3352953287214655</v>
@@ -14035,13 +14127,13 @@
         <v>0.48961786658503059</v>
       </c>
       <c r="AA129" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB129" s="0">
         <v>0.18829018331584305</v>
       </c>
-      <c r="AB129" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC129" s="0">
-        <v>0.33348591189087556</v>
+        <v>0.33348591189087551</v>
       </c>
       <c r="AD129" s="0">
         <v>0.10000000000000001</v>
@@ -14124,13 +14216,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z130" s="0">
-        <v>0.48356298359973537</v>
+        <v>0.48356298359973543</v>
       </c>
       <c r="AA130" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB130" s="0">
         <v>0.18644252583818394</v>
-      </c>
-      <c r="AB130" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC130" s="0">
         <v>0.33148849854595097</v>
@@ -14216,16 +14308,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z131" s="0">
-        <v>0.47725675147299612</v>
+        <v>0.47725675147299618</v>
       </c>
       <c r="AA131" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB131" s="0">
         <v>0.18446695033896365</v>
       </c>
-      <c r="AB131" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC131" s="0">
-        <v>0.32922185365613588</v>
+        <v>0.32922185365613593</v>
       </c>
       <c r="AD131" s="0">
         <v>0.10000000000000001</v>
@@ -14308,13 +14400,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z132" s="0">
-        <v>0.47040152868797425</v>
+        <v>0.47040152868797436</v>
       </c>
       <c r="AA132" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB132" s="0">
         <v>0.18260544048027846</v>
-      </c>
-      <c r="AB132" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC132" s="0">
         <v>0.32638379025992698</v>
@@ -14400,16 +14492,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z133" s="0">
-        <v>0.46469091129442874</v>
+        <v>0.4646909112944288</v>
       </c>
       <c r="AA133" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB133" s="0">
         <v>0.18095601946295031</v>
       </c>
-      <c r="AB133" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC133" s="0">
-        <v>0.32452071333685006</v>
+        <v>0.32452071333685012</v>
       </c>
       <c r="AD133" s="0">
         <v>0.10000000000000001</v>
@@ -14495,10 +14587,10 @@
         <v>0.45910921974373237</v>
       </c>
       <c r="AA134" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB134" s="0">
         <v>0.1793177277730722</v>
-      </c>
-      <c r="AB134" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC134" s="0">
         <v>0.32272763641377317</v>
@@ -14584,13 +14676,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z135" s="0">
-        <v>0.45359810016972246</v>
+        <v>0.45359810016972252</v>
       </c>
       <c r="AA135" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB135" s="0">
         <v>0.17777422465783213</v>
-      </c>
-      <c r="AB135" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC135" s="0">
         <v>0.32094514266010626</v>
@@ -14676,13 +14768,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z136" s="0">
-        <v>0.44815586316905937</v>
+        <v>0.44815586316905942</v>
       </c>
       <c r="AA136" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB136" s="0">
         <v>0.17611868702218589</v>
-      </c>
-      <c r="AB136" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC136" s="0">
         <v>0.319184466503106</v>
@@ -14771,13 +14863,13 @@
         <v>0.44276928317939801</v>
       </c>
       <c r="AA137" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB137" s="0">
         <v>0.17422037760885287</v>
       </c>
-      <c r="AB137" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC137" s="0">
-        <v>0.31744050022170961</v>
+        <v>0.31744050022170966</v>
       </c>
       <c r="AD137" s="0">
         <v>0.10000000000000001</v>
@@ -14860,13 +14952,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z138" s="0">
-        <v>0.43746068404287336</v>
+        <v>0.4374606840428733</v>
       </c>
       <c r="AA138" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB138" s="0">
         <v>0.17233893636071651</v>
-      </c>
-      <c r="AB138" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC138" s="0">
         <v>0.31571806817812392</v>
@@ -14952,13 +15044,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z139" s="0">
-        <v>0.43226294424662104</v>
+        <v>0.43226294424662098</v>
       </c>
       <c r="AA139" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB139" s="0">
         <v>0.17099329856816045</v>
-      </c>
-      <c r="AB139" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC139" s="0">
         <v>0.3140160695194123</v>
@@ -15047,13 +15139,13 @@
         <v>0.42711664331578597</v>
       </c>
       <c r="AA140" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB140" s="0">
         <v>0.16923936791956068</v>
       </c>
-      <c r="AB140" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC140" s="0">
-        <v>0.31233652971658543</v>
+        <v>0.31233652971658549</v>
       </c>
       <c r="AD140" s="0">
         <v>0.10000000000000001</v>
@@ -15136,16 +15228,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z141" s="0">
-        <v>0.42203904618349747</v>
+        <v>0.42203904618349741</v>
       </c>
       <c r="AA141" s="0">
-        <v>0.16734542922346007</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB141" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.16734542922346005</v>
       </c>
       <c r="AC141" s="0">
-        <v>0.31067889110105618</v>
+        <v>0.31067889110105623</v>
       </c>
       <c r="AD141" s="0">
         <v>0.10000000000000001</v>
@@ -15231,10 +15323,10 @@
         <v>0.41706643832926521</v>
       </c>
       <c r="AA142" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB142" s="0">
         <v>0.1658124394313602</v>
-      </c>
-      <c r="AB142" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC142" s="0">
         <v>0.30904744364421993</v>
@@ -15323,10 +15415,10 @@
         <v>0.41214173476548521</v>
       </c>
       <c r="AA143" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB143" s="0">
         <v>0.16388642280704507</v>
-      </c>
-      <c r="AB143" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC143" s="0">
         <v>0.30743305438771423</v>
@@ -15412,13 +15504,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z144" s="0">
-        <v>0.40731171953232931</v>
+        <v>0.4073117195323292</v>
       </c>
       <c r="AA144" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB144" s="0">
         <v>0.16231082501685423</v>
-      </c>
-      <c r="AB144" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC144" s="0">
         <v>0.30583409326834676</v>
@@ -15507,10 +15599,10 @@
         <v>0.40255475410140384</v>
       </c>
       <c r="AA145" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB145" s="0">
         <v>0.16057375121327602</v>
-      </c>
-      <c r="AB145" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC145" s="0">
         <v>0.30426250084562079</v>
@@ -15599,13 +15691,13 @@
         <v>0.397851411825554</v>
       </c>
       <c r="AA146" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB146" s="0">
         <v>0.15853640567696173</v>
       </c>
-      <c r="AB146" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC146" s="0">
-        <v>0.30270776096643165</v>
+        <v>0.3027077609664317</v>
       </c>
       <c r="AD146" s="0">
         <v>0.10000000000000001</v>
@@ -15688,16 +15780,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z147" s="0">
-        <v>0.3932627794324825</v>
+        <v>0.39326277943248256</v>
       </c>
       <c r="AA147" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB147" s="0">
         <v>0.15705746393017264</v>
       </c>
-      <c r="AB147" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC147" s="0">
-        <v>0.30117340823999506</v>
+        <v>0.30117340823999511</v>
       </c>
       <c r="AD147" s="0">
         <v>0.10000000000000001</v>
@@ -15780,16 +15872,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z148" s="0">
-        <v>0.38870643541823247</v>
+        <v>0.38870643541823252</v>
       </c>
       <c r="AA148" s="0">
-        <v>0.15501637719293385</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB148" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.15501637719293382</v>
       </c>
       <c r="AC148" s="0">
-        <v>0.29965112171116537</v>
+        <v>0.29965112171116542</v>
       </c>
       <c r="AD148" s="0">
         <v>0.10000000000000001</v>
@@ -15872,13 +15964,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z149" s="0">
-        <v>0.38426362066456188</v>
+        <v>0.38426362066456182</v>
       </c>
       <c r="AA149" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB149" s="0">
         <v>0.15361592564028068</v>
-      </c>
-      <c r="AB149" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC149" s="0">
         <v>0.29813830200425001</v>
@@ -15964,13 +16056,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z150" s="0">
-        <v>0.379854131786451</v>
+        <v>0.37985413178645094</v>
       </c>
       <c r="AA150" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB150" s="0">
         <v>0.15173050161960921</v>
-      </c>
-      <c r="AB150" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC150" s="0">
         <v>0.29663196837963607</v>
@@ -16059,10 +16151,10 @@
         <v>0.37551660946214555</v>
       </c>
       <c r="AA151" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB151" s="0">
         <v>0.14985346850353362</v>
-      </c>
-      <c r="AB151" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC151" s="0">
         <v>0.29513646465287235</v>
@@ -16148,13 +16240,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z152" s="0">
-        <v>0.37127070336384688</v>
+        <v>0.37127070336384682</v>
       </c>
       <c r="AA152" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB152" s="0">
         <v>0.14841529172187898</v>
-      </c>
-      <c r="AB152" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC152" s="0">
         <v>0.29363473413379537</v>
@@ -16243,10 +16335,10 @@
         <v>0.36705977857638622</v>
       </c>
       <c r="AA153" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB153" s="0">
         <v>0.14661588319183186</v>
-      </c>
-      <c r="AB153" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC153" s="0">
         <v>0.2921284258817759</v>
@@ -16335,10 +16427,10 @@
         <v>0.36291437282837175</v>
       </c>
       <c r="AA154" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB154" s="0">
         <v>0.1448572829953792</v>
-      </c>
-      <c r="AB154" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC154" s="0">
         <v>0.29061670799938083</v>
@@ -16427,13 +16519,13 @@
         <v>0.35882343247352799</v>
       </c>
       <c r="AA155" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB155" s="0">
         <v>0.14313158799148884</v>
       </c>
-      <c r="AB155" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC155" s="0">
-        <v>0.28908342662849229</v>
+        <v>0.28908342662849223</v>
       </c>
       <c r="AD155" s="0">
         <v>0.10000000000000001</v>
@@ -16519,13 +16611,13 @@
         <v>0.35479736268918649</v>
       </c>
       <c r="AA156" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB156" s="0">
         <v>0.14148788628740719</v>
       </c>
-      <c r="AB156" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC156" s="0">
-        <v>0.2875338900675401</v>
+        <v>0.28753389006754004</v>
       </c>
       <c r="AD156" s="0">
         <v>0.10000000000000001</v>
@@ -16611,10 +16703,10 @@
         <v>0.35080197727354362</v>
       </c>
       <c r="AA157" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB157" s="0">
         <v>0.1395302873478414</v>
-      </c>
-      <c r="AB157" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC157" s="0">
         <v>0.28596346399648626</v>
@@ -16700,16 +16792,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z158" s="0">
-        <v>0.34689469791278499</v>
+        <v>0.34689469791278504</v>
       </c>
       <c r="AA158" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB158" s="0">
         <v>0.13802792215849524</v>
       </c>
-      <c r="AB158" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC158" s="0">
-        <v>0.28435987864367379</v>
+        <v>0.28435987864367385</v>
       </c>
       <c r="AD158" s="0">
         <v>0.10000000000000001</v>
@@ -16795,10 +16887,10 @@
         <v>0.34303043610912276</v>
       </c>
       <c r="AA159" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB159" s="0">
         <v>0.13635661050700718</v>
-      </c>
-      <c r="AB159" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC159" s="0">
         <v>0.28272971088034421</v>
@@ -16884,13 +16976,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z160" s="0">
-        <v>0.33920729919770498</v>
+        <v>0.33920729919770504</v>
       </c>
       <c r="AA160" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB160" s="0">
         <v>0.13446997107629916</v>
-      </c>
-      <c r="AB160" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC160" s="0">
         <v>0.28107307424908567</v>
@@ -16976,16 +17068,16 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z161" s="0">
-        <v>0.33544604708829417</v>
+        <v>0.33544604708829423</v>
       </c>
       <c r="AA161" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB161" s="0">
         <v>0.13267806889912714</v>
       </c>
-      <c r="AB161" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC161" s="0">
-        <v>0.27937855281593388</v>
+        <v>0.27937855281593382</v>
       </c>
       <c r="AD161" s="0">
         <v>0.10000000000000001</v>
@@ -17071,10 +17163,10 @@
         <v>0.33175368556027912</v>
       </c>
       <c r="AA162" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB162" s="0">
         <v>0.13105786911013945</v>
-      </c>
-      <c r="AB162" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC162" s="0">
         <v>0.27764064415062811</v>
@@ -17163,10 +17255,10 @@
         <v>0.32809826997248143</v>
       </c>
       <c r="AA163" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB163" s="0">
         <v>0.12918475952362948</v>
-      </c>
-      <c r="AB163" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC163" s="0">
         <v>0.27586551358348554</v>
@@ -17255,10 +17347,10 @@
         <v>0.32452007787157222</v>
       </c>
       <c r="AA164" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB164" s="0">
         <v>0.12754748952713651</v>
-      </c>
-      <c r="AB164" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC164" s="0">
         <v>0.27404148951678375</v>
@@ -17347,10 +17439,10 @@
         <v>0.32097591290419392</v>
       </c>
       <c r="AA165" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB165" s="0">
         <v>0.12568747947100306</v>
-      </c>
-      <c r="AB165" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC165" s="0">
         <v>0.27216398782241757</v>
@@ -17436,13 +17528,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z166" s="0">
-        <v>0.31748906979568964</v>
+        <v>0.31748906979568958</v>
       </c>
       <c r="AA166" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB166" s="0">
         <v>0.12385608768746112</v>
-      </c>
-      <c r="AB166" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC166" s="0">
         <v>0.27022718210664465</v>
@@ -17528,13 +17620,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z167" s="0">
-        <v>0.3140560049796951</v>
+        <v>0.31405600497969516</v>
       </c>
       <c r="AA167" s="0">
-        <v>0.12198614778631957</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB167" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.12198614778631958</v>
       </c>
       <c r="AC167" s="0">
         <v>0.26823117876416908</v>
@@ -17620,13 +17712,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z168" s="0">
-        <v>0.31067565413133047</v>
+        <v>0.31067565413133058</v>
       </c>
       <c r="AA168" s="0">
-        <v>0.12010389785381435</v>
+        <v>0.10000000000000002</v>
       </c>
       <c r="AB168" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.12010389785381438</v>
       </c>
       <c r="AC168" s="0">
         <v>0.2661651420031399</v>
@@ -17715,10 +17807,10 @@
         <v>0.30737763871808588</v>
       </c>
       <c r="AA169" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB169" s="0">
         <v>0.1184873932767251</v>
-      </c>
-      <c r="AB169" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC169" s="0">
         <v>0.26402329631025556</v>
@@ -17804,13 +17896,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z170" s="0">
-        <v>0.3041148047753246</v>
+        <v>0.30411480477532465</v>
       </c>
       <c r="AA170" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB170" s="0">
         <v>0.11665663456698032</v>
-      </c>
-      <c r="AB170" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC170" s="0">
         <v>0.26180633113383406</v>
@@ -17896,13 +17988,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z171" s="0">
-        <v>0.30089512569034688</v>
+        <v>0.30089512569034693</v>
       </c>
       <c r="AA171" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB171" s="0">
         <v>0.11469417459796936</v>
-      </c>
-      <c r="AB171" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC171" s="0">
         <v>0.25950871904509781</v>
@@ -17991,10 +18083,10 @@
         <v>0.29775229709284567</v>
       </c>
       <c r="AA172" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB172" s="0">
         <v>0.11286191415991845</v>
-      </c>
-      <c r="AB172" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC172" s="0">
         <v>0.2571354856233824</v>
@@ -18080,13 +18172,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z173" s="0">
-        <v>0.29469075209757467</v>
+        <v>0.29469075209757473</v>
       </c>
       <c r="AA173" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB173" s="0">
         <v>0.1111945096087719</v>
-      </c>
-      <c r="AB173" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC173" s="0">
         <v>0.25468123645762947</v>
@@ -18172,13 +18264,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z174" s="0">
-        <v>0.29167129110055301</v>
+        <v>0.29167129110055307</v>
       </c>
       <c r="AA174" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB174" s="0">
         <v>0.10932921998561201</v>
-      </c>
-      <c r="AB174" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC174" s="0">
         <v>0.25214637458623462</v>
@@ -18264,13 +18356,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z175" s="0">
-        <v>0.28870924447029112</v>
+        <v>0.28870924447029117</v>
       </c>
       <c r="AA175" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB175" s="0">
         <v>0.10738650701289236</v>
-      </c>
-      <c r="AB175" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC175" s="0">
         <v>0.24953074323934971</v>
@@ -18359,13 +18451,13 @@
         <v>0.28583031132271641</v>
       </c>
       <c r="AA176" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB176" s="0">
         <v>0.10557749212643593</v>
       </c>
-      <c r="AB176" s="0">
-        <v>0.10000000000000001</v>
-      </c>
       <c r="AC176" s="0">
-        <v>0.24683411674685066</v>
+        <v>0.24683411674685068</v>
       </c>
       <c r="AD176" s="0">
         <v>0.10000000000000001</v>
@@ -18451,10 +18543,10 @@
         <v>0.28302092812891672</v>
       </c>
       <c r="AA177" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB177" s="0">
         <v>0.10375337441431139</v>
-      </c>
-      <c r="AB177" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC177" s="0">
         <v>0.24406202511870181</v>
@@ -18540,13 +18632,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="Z178" s="0">
-        <v>0.28029733985770849</v>
+        <v>0.28029733985770855</v>
       </c>
       <c r="AA178" s="0">
-        <v>0.10204192728372136</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="AB178" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.10204192728372137</v>
       </c>
       <c r="AC178" s="0">
         <v>0.24121436978241267</v>
@@ -18635,10 +18727,10 @@
         <v>0.2776453579840415</v>
       </c>
       <c r="AA179" s="0">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="AB179" s="0">
         <v>0.10028794242511167</v>
-      </c>
-      <c r="AB179" s="0">
-        <v>0.10000000000000001</v>
       </c>
       <c r="AC179" s="0">
         <v>0.238302020794119</v>
@@ -18724,7 +18816,7 @@
         <v>0.10347025226231726</v>
       </c>
       <c r="Z180" s="0">
-        <v>0.27507442404205995</v>
+        <v>0.27507442404206001</v>
       </c>
       <c r="AA180" s="0">
         <v>0.10000000000000001</v>
@@ -18816,7 +18908,7 @@
         <v>0.10757031370095112</v>
       </c>
       <c r="Z181" s="0">
-        <v>0.27258640718245108</v>
+        <v>0.27258640718245114</v>
       </c>
       <c r="AA181" s="0">
         <v>0.10000000000000001</v>
@@ -19181,10 +19273,10 @@
         <v>0</v>
       </c>
       <c r="Y185" s="0">
-        <v>0.12298347356084732</v>
+        <v>0.12298347356084734</v>
       </c>
       <c r="Z185" s="0">
-        <v>0.26346492452088965</v>
+        <v>0.2634649245208896</v>
       </c>
       <c r="AA185" s="0">
         <v>0.10000000000000001</v>
@@ -19365,7 +19457,7 @@
         <v>0</v>
       </c>
       <c r="Y187" s="0">
-        <v>0.13010408691633865</v>
+        <v>0.13010408691633862</v>
       </c>
       <c r="Z187" s="0">
         <v>0.25940612101905347</v>
@@ -19460,7 +19552,7 @@
         <v>0.13332790840933928</v>
       </c>
       <c r="Z188" s="0">
-        <v>0.25751265498163678</v>
+        <v>0.25751265498163672</v>
       </c>
       <c r="AA188" s="0">
         <v>0.10000000000000001</v>
@@ -19549,10 +19641,10 @@
         <v>0</v>
       </c>
       <c r="Y189" s="0">
-        <v>0.13648058737135757</v>
+        <v>0.1364805873713576</v>
       </c>
       <c r="Z189" s="0">
-        <v>0.25569773667704837</v>
+        <v>0.25569773667704832</v>
       </c>
       <c r="AA189" s="0">
         <v>0.10000000000000001</v>
@@ -19733,7 +19825,7 @@
         <v>0</v>
       </c>
       <c r="Y191" s="0">
-        <v>0.14250609369852957</v>
+        <v>0.14250609369852954</v>
       </c>
       <c r="Z191" s="0">
         <v>0.25231269453989968</v>
@@ -19825,7 +19917,7 @@
         <v>0</v>
       </c>
       <c r="Y192" s="0">
-        <v>0.14507456712502026</v>
+        <v>0.14507456712502023</v>
       </c>
       <c r="Z192" s="0">
         <v>0.25075420988412211</v>
@@ -19920,7 +20012,7 @@
         <v>0.14764246179555524</v>
       </c>
       <c r="Z193" s="0">
-        <v>0.24926615821948214</v>
+        <v>0.2492661582194822</v>
       </c>
       <c r="AA193" s="0">
         <v>0.10000000000000001</v>
@@ -20104,7 +20196,7 @@
         <v>0.1522059927072969</v>
       </c>
       <c r="Z195" s="0">
-        <v>0.24652992916154454</v>
+        <v>0.24652992916154456</v>
       </c>
       <c r="AA195" s="0">
         <v>0.10000000000000001</v>
@@ -20840,7 +20932,7 @@
         <v>0.16599536846957377</v>
       </c>
       <c r="Z203" s="0">
-        <v>0.2382295302844552</v>
+        <v>0.23822953028445523</v>
       </c>
       <c r="AA203" s="0">
         <v>0.10000000000000001</v>
@@ -22585,10 +22677,10 @@
         <v>0</v>
       </c>
       <c r="Y222" s="0">
-        <v>0.17838867746783324</v>
+        <v>0.17838867746783321</v>
       </c>
       <c r="Z222" s="0">
-        <v>0.228295492038257</v>
+        <v>0.22829549203825703</v>
       </c>
       <c r="AA222" s="0">
         <v>0.10000000000000001</v>
@@ -22597,7 +22689,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC222" s="0">
-        <v>0.13297921460868609</v>
+        <v>0.13297921460868611</v>
       </c>
       <c r="AD222" s="0">
         <v>0.10000000000000001</v>
@@ -22772,7 +22864,7 @@
         <v>0.17869285715970998</v>
       </c>
       <c r="Z224" s="0">
-        <v>0.22763073303576084</v>
+        <v>0.22763073303576081</v>
       </c>
       <c r="AA224" s="0">
         <v>0.10000000000000001</v>
@@ -22864,7 +22956,7 @@
         <v>0.1788354262846602</v>
       </c>
       <c r="Z225" s="0">
-        <v>0.22732314608377144</v>
+        <v>0.22732314608377147</v>
       </c>
       <c r="AA225" s="0">
         <v>0.10000000000000001</v>
@@ -22956,7 +23048,7 @@
         <v>0.17890234052363929</v>
       </c>
       <c r="Z226" s="0">
-        <v>0.22701435660092309</v>
+        <v>0.22701435660092306</v>
       </c>
       <c r="AA226" s="0">
         <v>0.10000000000000001</v>
@@ -23048,7 +23140,7 @@
         <v>0.17895566374097835</v>
       </c>
       <c r="Z227" s="0">
-        <v>0.22670786645505428</v>
+        <v>0.22670786645505431</v>
       </c>
       <c r="AA227" s="0">
         <v>0.10000000000000001</v>
@@ -23140,7 +23232,7 @@
         <v>0.17898326218417784</v>
       </c>
       <c r="Z228" s="0">
-        <v>0.22641294171431281</v>
+        <v>0.22641294171431278</v>
       </c>
       <c r="AA228" s="0">
         <v>0.10000000000000001</v>
@@ -23232,7 +23324,7 @@
         <v>0.17899480584182209</v>
       </c>
       <c r="Z229" s="0">
-        <v>0.22614216558176276</v>
+        <v>0.22614216558176278</v>
       </c>
       <c r="AA229" s="0">
         <v>0.10000000000000001</v>
@@ -23324,7 +23416,7 @@
         <v>0.17897802987546849</v>
       </c>
       <c r="Z230" s="0">
-        <v>0.22587680935963106</v>
+        <v>0.22587680935963103</v>
       </c>
       <c r="AA230" s="0">
         <v>0.10000000000000001</v>
@@ -23416,7 +23508,7 @@
         <v>0.17893873727810858</v>
       </c>
       <c r="Z231" s="0">
-        <v>0.22562381752864516</v>
+        <v>0.22562381752864519</v>
       </c>
       <c r="AA231" s="0">
         <v>0.10000000000000001</v>
@@ -23508,7 +23600,7 @@
         <v>0.17889754707754563</v>
       </c>
       <c r="Z232" s="0">
-        <v>0.22538346697910949</v>
+        <v>0.22538346697910952</v>
       </c>
       <c r="AA232" s="0">
         <v>0.10000000000000001</v>
@@ -23600,7 +23692,7 @@
         <v>0.17881026322875548</v>
       </c>
       <c r="Z233" s="0">
-        <v>0.22516591792074839</v>
+        <v>0.22516591792074836</v>
       </c>
       <c r="AA233" s="0">
         <v>0.10000000000000001</v>
@@ -23784,7 +23876,7 @@
         <v>0.178659174147974</v>
       </c>
       <c r="Z235" s="0">
-        <v>0.22474260849722211</v>
+        <v>0.22474260849722213</v>
       </c>
       <c r="AA235" s="0">
         <v>0.10000000000000001</v>
@@ -24244,7 +24336,7 @@
         <v>0.17830828306648386</v>
       </c>
       <c r="Z240" s="0">
-        <v>0.22404239751147489</v>
+        <v>0.22404239751147492</v>
       </c>
       <c r="AA240" s="0">
         <v>0.10000000000000001</v>
@@ -24336,7 +24428,7 @@
         <v>0.17825096193965392</v>
       </c>
       <c r="Z241" s="0">
-        <v>0.22398816362574978</v>
+        <v>0.2239881636257498</v>
       </c>
       <c r="AA241" s="0">
         <v>0.10000000000000001</v>
@@ -24704,7 +24796,7 @@
         <v>0.17832300468518922</v>
       </c>
       <c r="Z245" s="0">
-        <v>0.22405781281321013</v>
+        <v>0.22405781281321011</v>
       </c>
       <c r="AA245" s="0">
         <v>0.10000000000000001</v>
@@ -24793,10 +24885,10 @@
         <v>0</v>
       </c>
       <c r="Y246" s="0">
-        <v>0.17841010407173649</v>
+        <v>0.17841010407173652</v>
       </c>
       <c r="Z246" s="0">
-        <v>0.22415927842934769</v>
+        <v>0.22415927842934766</v>
       </c>
       <c r="AA246" s="0">
         <v>0.10000000000000001</v>
@@ -25256,7 +25348,7 @@
         <v>0.17893023202779962</v>
       </c>
       <c r="Z251" s="0">
-        <v>0.22527932395035585</v>
+        <v>0.22527932395035583</v>
       </c>
       <c r="AA251" s="0">
         <v>0.10000000000000001</v>
@@ -25348,7 +25440,7 @@
         <v>0.17911465162423287</v>
       </c>
       <c r="Z252" s="0">
-        <v>0.22559781359051451</v>
+        <v>0.22559781359051453</v>
       </c>
       <c r="AA252" s="0">
         <v>0.10000000000000001</v>
@@ -25437,10 +25529,10 @@
         <v>0</v>
       </c>
       <c r="Y253" s="0">
-        <v>0.17924407386023314</v>
+        <v>0.17924407386023311</v>
       </c>
       <c r="Z253" s="0">
-        <v>0.22596912432347377</v>
+        <v>0.2259691243234738</v>
       </c>
       <c r="AA253" s="0">
         <v>0.10000000000000001</v>
@@ -25449,7 +25541,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC253" s="0">
-        <v>0.11711320912812827</v>
+        <v>0.11711320912812828</v>
       </c>
       <c r="AD253" s="0">
         <v>0.10000000000000001</v>
@@ -25532,7 +25624,7 @@
         <v>0.17937267163243995</v>
       </c>
       <c r="Z254" s="0">
-        <v>0.22636701250248789</v>
+        <v>0.22636701250248786</v>
       </c>
       <c r="AA254" s="0">
         <v>0.10000000000000001</v>
@@ -25624,7 +25716,7 @@
         <v>0.17948138101220024</v>
       </c>
       <c r="Z255" s="0">
-        <v>0.22680860372420503</v>
+        <v>0.22680860372420505</v>
       </c>
       <c r="AA255" s="0">
         <v>0.10000000000000001</v>
@@ -25808,7 +25900,7 @@
         <v>0.17974502009159726</v>
       </c>
       <c r="Z257" s="0">
-        <v>0.22774199713779328</v>
+        <v>0.22774199713779325</v>
       </c>
       <c r="AA257" s="0">
         <v>0.10000000000000001</v>
@@ -25900,7 +25992,7 @@
         <v>0.17985233484262478</v>
       </c>
       <c r="Z258" s="0">
-        <v>0.22824984782724328</v>
+        <v>0.22824984782724325</v>
       </c>
       <c r="AA258" s="0">
         <v>0.10000000000000001</v>
@@ -25989,10 +26081,10 @@
         <v>0</v>
       </c>
       <c r="Y259" s="0">
-        <v>0.17995516400447475</v>
+        <v>0.17995516400447478</v>
       </c>
       <c r="Z259" s="0">
-        <v>0.22876571781285218</v>
+        <v>0.22876571781285224</v>
       </c>
       <c r="AA259" s="0">
         <v>0.10000000000000001</v>
@@ -26001,7 +26093,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC259" s="0">
-        <v>0.1183081955195754</v>
+        <v>0.11830819551957537</v>
       </c>
       <c r="AD259" s="0">
         <v>0.10000000000000001</v>
@@ -26277,7 +26369,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC262" s="0">
-        <v>0.11903921402602918</v>
+        <v>0.1190392140260292</v>
       </c>
       <c r="AD262" s="0">
         <v>0.10000000000000001</v>
@@ -26357,7 +26449,7 @@
         <v>0</v>
       </c>
       <c r="Y263" s="0">
-        <v>0.18016832424218612</v>
+        <v>0.1801683242421861</v>
       </c>
       <c r="Z263" s="0">
         <v>0.2309810219331542</v>
@@ -26728,7 +26820,7 @@
         <v>0.1801984156143662</v>
       </c>
       <c r="Z267" s="0">
-        <v>0.23332931664219053</v>
+        <v>0.23332931664219056</v>
       </c>
       <c r="AA267" s="0">
         <v>0.10000000000000001</v>
@@ -27553,10 +27645,10 @@
         <v>0</v>
       </c>
       <c r="Y276" s="0">
-        <v>0.18030363101985034</v>
+        <v>0.18030363101985039</v>
       </c>
       <c r="Z276" s="0">
-        <v>0.23889794813727466</v>
+        <v>0.23889794813727463</v>
       </c>
       <c r="AA276" s="0">
         <v>0.10000000000000001</v>
@@ -27565,7 +27657,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC276" s="0">
-        <v>0.12250123825325543</v>
+        <v>0.12250123825325542</v>
       </c>
       <c r="AD276" s="0">
         <v>0.10000000000000001</v>
@@ -28025,7 +28117,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC281" s="0">
-        <v>0.12324077984263222</v>
+        <v>0.12324077984263224</v>
       </c>
       <c r="AD281" s="0">
         <v>0.10000000000000001</v>
@@ -28117,7 +28209,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC282" s="0">
-        <v>0.12335842648762142</v>
+        <v>0.12335842648762141</v>
       </c>
       <c r="AD282" s="0">
         <v>0.10000000000000001</v>
@@ -28209,7 +28301,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC283" s="0">
-        <v>0.12344240403954171</v>
+        <v>0.12344240403954172</v>
       </c>
       <c r="AD283" s="0">
         <v>0.10000000000000001</v>
@@ -28301,7 +28393,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC284" s="0">
-        <v>0.12352828551719319</v>
+        <v>0.12352828551719318</v>
       </c>
       <c r="AD284" s="0">
         <v>0.10000000000000001</v>
@@ -28761,7 +28853,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC289" s="0">
-        <v>0.12360496038244367</v>
+        <v>0.12360496038244369</v>
       </c>
       <c r="AD289" s="0">
         <v>0.10000000000000001</v>
@@ -28853,7 +28945,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC290" s="0">
-        <v>0.12356133629276483</v>
+        <v>0.12356133629276482</v>
       </c>
       <c r="AD290" s="0">
         <v>0.10000000000000001</v>
@@ -28945,7 +29037,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC291" s="0">
-        <v>0.1234961734473586</v>
+        <v>0.12349617344735858</v>
       </c>
       <c r="AD291" s="0">
         <v>0.10000000000000001</v>
@@ -29129,7 +29221,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC293" s="0">
-        <v>0.12331820729897085</v>
+        <v>0.12331820729897086</v>
       </c>
       <c r="AD293" s="0">
         <v>0.10000000000000001</v>
@@ -29393,7 +29485,7 @@
         <v>0</v>
       </c>
       <c r="Y296" s="0">
-        <v>0.18424990849147338</v>
+        <v>0.18424990849147341</v>
       </c>
       <c r="Z296" s="0">
         <v>0.24561350793474507</v>
@@ -29405,7 +29497,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC296" s="0">
-        <v>0.12298974576050932</v>
+        <v>0.12298974576050935</v>
       </c>
       <c r="AD296" s="0">
         <v>0.10000000000000001</v>
@@ -29485,10 +29577,10 @@
         <v>0</v>
       </c>
       <c r="Y297" s="0">
-        <v>0.18470047853577443</v>
+        <v>0.1847004785357744</v>
       </c>
       <c r="Z297" s="0">
-        <v>0.2456419335918551</v>
+        <v>0.24564193359185513</v>
       </c>
       <c r="AA297" s="0">
         <v>0.10000000000000001</v>
@@ -29497,7 +29589,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC297" s="0">
-        <v>0.12283441321584175</v>
+        <v>0.12283441321584179</v>
       </c>
       <c r="AD297" s="0">
         <v>0.10000000000000001</v>
@@ -29577,7 +29669,7 @@
         <v>0</v>
       </c>
       <c r="Y298" s="0">
-        <v>0.18509108485208342</v>
+        <v>0.18509108485208345</v>
       </c>
       <c r="Z298" s="0">
         <v>0.24571097720553348</v>
@@ -30500,7 +30592,7 @@
         <v>0.19078674594318226</v>
       </c>
       <c r="Z308" s="0">
-        <v>0.24506065121597301</v>
+        <v>0.24506065121597304</v>
       </c>
       <c r="AA308" s="0">
         <v>0.10000000000000001</v>
@@ -30868,7 +30960,7 @@
         <v>0.19342535262125116</v>
       </c>
       <c r="Z312" s="0">
-        <v>0.24441247546017475</v>
+        <v>0.24441247546017478</v>
       </c>
       <c r="AA312" s="0">
         <v>0.10000000000000001</v>
@@ -30960,7 +31052,7 @@
         <v>0.19418552651365809</v>
       </c>
       <c r="Z313" s="0">
-        <v>0.24418610529286672</v>
+        <v>0.24418610529286669</v>
       </c>
       <c r="AA313" s="0">
         <v>0.10000000000000001</v>
@@ -31049,7 +31141,7 @@
         <v>0</v>
       </c>
       <c r="Y314" s="0">
-        <v>0.19494739788000071</v>
+        <v>0.19494739788000073</v>
       </c>
       <c r="Z314" s="0">
         <v>0.24392402464281487</v>
@@ -31233,7 +31325,7 @@
         <v>0</v>
       </c>
       <c r="Y316" s="0">
-        <v>0.19650689001137223</v>
+        <v>0.19650689001137225</v>
       </c>
       <c r="Z316" s="0">
         <v>0.24346939258538192</v>
@@ -31328,7 +31420,7 @@
         <v>0.19737644691231429</v>
       </c>
       <c r="Z317" s="0">
-        <v>0.24317509959583022</v>
+        <v>0.24317509959583025</v>
       </c>
       <c r="AA317" s="0">
         <v>0.10000000000000001</v>
@@ -31420,7 +31512,7 @@
         <v>0.19822469270096651</v>
       </c>
       <c r="Z318" s="0">
-        <v>0.24292787637116758</v>
+        <v>0.24292787637116756</v>
       </c>
       <c r="AA318" s="0">
         <v>0.10000000000000001</v>
@@ -31512,7 +31604,7 @@
         <v>0.19904045987732424</v>
       </c>
       <c r="Z319" s="0">
-        <v>0.24271291338070375</v>
+        <v>0.24271291338070378</v>
       </c>
       <c r="AA319" s="0">
         <v>0.10000000000000001</v>
@@ -31696,7 +31788,7 @@
         <v>0.20058183177218253</v>
       </c>
       <c r="Z321" s="0">
-        <v>0.24236622261445459</v>
+        <v>0.24236622261445456</v>
       </c>
       <c r="AA321" s="0">
         <v>0.10000000000000001</v>
@@ -31788,7 +31880,7 @@
         <v>0.20141990121961975</v>
       </c>
       <c r="Z322" s="0">
-        <v>0.24222632625235191</v>
+        <v>0.24222632625235188</v>
       </c>
       <c r="AA322" s="0">
         <v>0.10000000000000001</v>
@@ -31969,10 +32061,10 @@
         <v>0</v>
       </c>
       <c r="Y324" s="0">
-        <v>0.20299483597862356</v>
+        <v>0.20299483597862358</v>
       </c>
       <c r="Z324" s="0">
-        <v>0.24201329889069811</v>
+        <v>0.24201329889069809</v>
       </c>
       <c r="AA324" s="0">
         <v>0.10000000000000001</v>
@@ -31981,7 +32073,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC324" s="0">
-        <v>0.11715201155657566</v>
+        <v>0.11715201155657562</v>
       </c>
       <c r="AD324" s="0">
         <v>0.10000000000000001</v>
@@ -32889,10 +32981,10 @@
         <v>0</v>
       </c>
       <c r="Y334" s="0">
-        <v>0.20928997166149071</v>
+        <v>0.20928997166149074</v>
       </c>
       <c r="Z334" s="0">
-        <v>0.24483675091126006</v>
+        <v>0.24483675091126003</v>
       </c>
       <c r="AA334" s="0">
         <v>0.10000000000000001</v>
@@ -32901,7 +32993,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC334" s="0">
-        <v>0.1177657462394097</v>
+        <v>0.11776574623940968</v>
       </c>
       <c r="AD334" s="0">
         <v>0.10000000000000001</v>
@@ -32981,10 +33073,10 @@
         <v>0</v>
       </c>
       <c r="Y335" s="0">
-        <v>0.20963150607532161</v>
+        <v>0.20963150607532163</v>
       </c>
       <c r="Z335" s="0">
-        <v>0.24561729561612827</v>
+        <v>0.24561729561612825</v>
       </c>
       <c r="AA335" s="0">
         <v>0.10000000000000001</v>
@@ -32993,7 +33085,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC335" s="0">
-        <v>0.11808831351708132</v>
+        <v>0.11808831351708134</v>
       </c>
       <c r="AD335" s="0">
         <v>0.10000000000000001</v>
@@ -33165,10 +33257,10 @@
         <v>0</v>
       </c>
       <c r="Y337" s="0">
-        <v>0.21013492739045292</v>
+        <v>0.21013492739045295</v>
       </c>
       <c r="Z337" s="0">
-        <v>0.247641702166565</v>
+        <v>0.24764170216656498</v>
       </c>
       <c r="AA337" s="0">
         <v>0.10000000000000001</v>
@@ -33177,7 +33269,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC337" s="0">
-        <v>0.11898320423502812</v>
+        <v>0.11898320423502809</v>
       </c>
       <c r="AD337" s="0">
         <v>0.10000000000000001</v>
@@ -33441,10 +33533,10 @@
         <v>0</v>
       </c>
       <c r="Y340" s="0">
-        <v>0.21029152144137458</v>
+        <v>0.21029152144137456</v>
       </c>
       <c r="Z340" s="0">
-        <v>0.25177115761743379</v>
+        <v>0.25177115761743385</v>
       </c>
       <c r="AA340" s="0">
         <v>0.10000000000000001</v>
@@ -33533,7 +33625,7 @@
         <v>0</v>
       </c>
       <c r="Y341" s="0">
-        <v>0.2101583103169018</v>
+        <v>0.21015831031690174</v>
       </c>
       <c r="Z341" s="0">
         <v>0.25333949845068021</v>
@@ -33545,7 +33637,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC341" s="0">
-        <v>0.12159997142928979</v>
+        <v>0.12159997142928977</v>
       </c>
       <c r="AD341" s="0">
         <v>0.10000000000000001</v>
@@ -33821,7 +33913,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="AC344" s="0">
-        <v>0.12442465550217195</v>
+        <v>0.12442465550217197</v>
       </c>
       <c r="AD344" s="0">
         <v>0.10000000000000001</v>
@@ -33901,10 +33993,10 @@
         <v>0</v>
       </c>
       <c r="Y345" s="0">
-        <v>0.20840909114892256</v>
+        <v>0.20840909114892253</v>
       </c>
       <c r="Z345" s="0">
-        <v>0.26156555256655334</v>
+        <v>0.26156555256655339</v>
       </c>
       <c r="AA345" s="0">
         <v>0.10000000000000001</v>
@@ -33993,7 +34085,7 @@
         <v>0</v>
       </c>
       <c r="Y346" s="0">
-        <v>0.20762946595873907</v>
+        <v>0.20762946595873905</v>
       </c>
       <c r="Z346" s="0">
         <v>0.26413632123100833</v>
@@ -34177,10 +34269,10 @@
         <v>0</v>
       </c>
       <c r="Y348" s="0">
-        <v>0.20555981677477375</v>
+        <v>0.20555981677477372</v>
       </c>
       <c r="Z348" s="0">
-        <v>0.26996115930458081</v>
+        <v>0.26996115930458087</v>
       </c>
       <c r="AA348" s="0">
         <v>0.10000000000000001</v>
@@ -34269,10 +34361,10 @@
         <v>0</v>
       </c>
       <c r="Y349" s="0">
-        <v>0.20454302396204219</v>
+        <v>0.20454302396204216</v>
       </c>
       <c r="Z349" s="0">
-        <v>0.27266216123073195</v>
+        <v>0.272662161230732</v>
       </c>
       <c r="AA349" s="0">
         <v>0.10000000000000001</v>
@@ -34361,7 +34453,7 @@
         <v>0</v>
       </c>
       <c r="Y350" s="0">
-        <v>0.20320817201356364</v>
+        <v>0.20320817201356361</v>
       </c>
       <c r="Z350" s="0">
         <v>0.27584984953905983</v>
@@ -34640,7 +34732,7 @@
         <v>0.19882358004879511</v>
       </c>
       <c r="Z353" s="0">
-        <v>0.28545158384632013</v>
+        <v>0.28545158384632019</v>
       </c>
       <c r="AA353" s="0">
         <v>0.10000000000000001</v>
@@ -35100,7 +35192,7 @@
         <v>0.18791678722381136</v>
       </c>
       <c r="Z358" s="0">
-        <v>0.30570781412347531</v>
+        <v>0.30570781412347536</v>
       </c>
       <c r="AA358" s="0">
         <v>0.10000000000000001</v>
@@ -35192,7 +35284,7 @@
         <v>0.18529741453559259</v>
       </c>
       <c r="Z359" s="0">
-        <v>0.31004109282226072</v>
+        <v>0.31004109282226067</v>
       </c>
       <c r="AA359" s="0">
         <v>0.10000000000000001</v>
@@ -35284,7 +35376,7 @@
         <v>0.18256692902185326</v>
       </c>
       <c r="Z360" s="0">
-        <v>0.31456950381630955</v>
+        <v>0.3145695038163096</v>
       </c>
       <c r="AA360" s="0">
         <v>0.10000000000000001</v>
@@ -35465,7 +35557,7 @@
         <v>0</v>
       </c>
       <c r="Y362" s="0">
-        <v>0.17698841486691094</v>
+        <v>0.17698841486691091</v>
       </c>
       <c r="Z362" s="0">
         <v>0.32339390803646673</v>

</xml_diff>